<commit_message>
Update js file with more data from excel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\3DVista\3DVista\BC Dufour\חומרי כרטיסייה\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guysh\ParserTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{82744D8D-D9B4-43F2-BA25-B9637BB41965}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D005D68-961A-42A9-9ADC-D07B746691A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
   <si>
     <t>DC ELECTRIC PANEL</t>
   </si>
@@ -101,13 +101,121 @@
   </si>
   <si>
     <t>http://ec2-18-224-43-229.us-east-2.compute.amazonaws.com:3200/product/3947471850314</t>
+  </si>
+  <si>
+    <t xml:space="preserve">                                         Troubleshooting</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Diagram</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> User Manuel</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Checklist</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Photo</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/volvo/um/Volvo-penta-D2-75_UM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/volvo/ts/Volvo-penta-D2-75_TS1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/volvo/photo/Volvo-penta-D2-75_photo.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/volvo/checklist/Volvo-penta-D2-75_Chek-List.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/DC_ELECTRIC_PANEL/ts/DC_Elc._Panel_VDO_TS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/DC_ELECTRIC_PANEL/diagram/DC_Elc._Panel_Diagram.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/DC_ELECTRIC_PANEL/photo/DC_Elc._Panel_photo.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_ELECTRIC_PANEL/ts/AC_Elc._Panel_VDO_TS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_ELECTRIC_PANEL/diagram/AC_Elc._Panel_Diagram.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_ELECTRIC_PANEL/photo/AC_Elc._Panel_photo.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_PANEL/ts/Dometic_AC_TS1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_PANEL/diagram/Dometic_AC_diagram.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_PANEL/photo/Dometic-AC_photo.jpg</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/AC_PANEL/um/Dometic_AC_UM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Compass/ts/Olympic_135_TS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Compass/diagram/Olympic_135_diagram.jpg</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Compass/um/Olympic_135_UM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Compass/photo/olympic_135_Photo.jpg</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Jib_Winch/ts/Lewmar_50ST_EVO_Electric_Winch_12_TS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Jib_Winch/diagram/Lewmar_50ST_EVO_Electric_Winch_12_Diagram.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Jib_Winch/um/Lewmar_50ST_EVo_Electric_Winch_12_UM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Jib_Winch/photo/Lewmar_50ST_Electric_Winch_12_photo1.jpg</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Fusion_Apollo/ts/Fusion_MS_RA_770_TS.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Fusion_Apollo/diagram/Fusion_MS_RA_770_DIAGRAM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Fusion_Apollo/um/Fusion_MS_RA_770_UM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/Fusion_Apollo/photo/Fusion_MS_RA_770_photo.jpg</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/fischr/ts/Generator-fischer-panda-8000i-pms_TS1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/fischr/diagram/Generator-fischer-panda-8000i-pms_Diagram.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/fischr/um/Generator-fischer-panda-8000i-pms_UM.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/fischr/checklist/Generato-fischer-panda-8000i-pms_check-list.pdf</t>
+  </si>
+  <si>
+    <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/fischr/photo/Generator-fischer-panda-8000i-pms_Photo.pdf</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -135,6 +243,13 @@
     </font>
     <font>
       <sz val="8"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -193,15 +308,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -215,6 +323,12 @@
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -434,167 +548,371 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:BC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.44140625" style="2"/>
-    <col min="2" max="2" width="34.21875" style="3" customWidth="1"/>
-    <col min="3" max="3" width="114.5546875" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="58" style="2" customWidth="1"/>
-    <col min="6" max="16384" width="14.44140625" style="2"/>
+    <col min="1" max="1" width="14.44140625" style="3"/>
+    <col min="2" max="2" width="34.21875" style="4" customWidth="1"/>
+    <col min="3" max="3" width="114.5546875" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="58" style="3" customWidth="1"/>
+    <col min="5" max="5" width="76.77734375" style="3" customWidth="1"/>
+    <col min="6" max="6" width="96.88671875" style="3" customWidth="1"/>
+    <col min="7" max="7" width="106.44140625" style="3" customWidth="1"/>
+    <col min="8" max="8" width="100.88671875" style="3" customWidth="1"/>
+    <col min="9" max="9" width="110.44140625" style="3" customWidth="1"/>
+    <col min="10" max="10" width="99.33203125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="14.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" s="1" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:55" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C1" s="5" t="s">
+      <c r="C1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="D1" s="5" t="s">
+      <c r="D1" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="E1" s="5" t="s">
+      <c r="E1" s="2" t="s">
         <v>14</v>
       </c>
+      <c r="F1" s="9" t="s">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="H1" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="I1" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J1" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" s="2"/>
+      <c r="L1" s="2"/>
+      <c r="M1" s="2"/>
+      <c r="N1" s="2"/>
+      <c r="O1" s="2"/>
+      <c r="P1" s="2"/>
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2"/>
+      <c r="S1" s="2"/>
+      <c r="T1" s="2"/>
+      <c r="U1" s="2"/>
+      <c r="V1" s="2"/>
+      <c r="W1" s="2"/>
+      <c r="X1" s="2"/>
+      <c r="Y1" s="2"/>
+      <c r="Z1" s="2"/>
+      <c r="AA1" s="2"/>
+      <c r="AB1" s="2"/>
+      <c r="AC1" s="2"/>
+      <c r="AD1" s="2"/>
+      <c r="AE1" s="2"/>
+      <c r="AF1" s="2"/>
+      <c r="AG1" s="2"/>
+      <c r="AH1" s="2"/>
+      <c r="AI1" s="2"/>
+      <c r="AJ1" s="2"/>
+      <c r="AK1" s="2"/>
+      <c r="AL1" s="2"/>
+      <c r="AM1" s="2"/>
+      <c r="AN1" s="2"/>
+      <c r="AO1" s="2"/>
+      <c r="AP1" s="2"/>
+      <c r="AQ1" s="2"/>
+      <c r="AR1" s="2"/>
+      <c r="AS1" s="2"/>
+      <c r="AT1" s="2"/>
+      <c r="AU1" s="2"/>
+      <c r="AV1" s="2"/>
+      <c r="AW1" s="2"/>
+      <c r="AX1" s="2"/>
+      <c r="AY1" s="2"/>
+      <c r="AZ1" s="2"/>
+      <c r="BA1" s="2"/>
+      <c r="BB1" s="2"/>
+      <c r="BC1" s="3"/>
     </row>
-    <row r="2" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="6">
+    <row r="2" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="3">
         <v>1009</v>
       </c>
-      <c r="B2" s="7" t="s">
+      <c r="B2" s="4" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="10" t="s">
+      <c r="D2" s="7" t="s">
         <v>18</v>
       </c>
-      <c r="E2" s="6" t="s">
+      <c r="E2" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F2" s="6" t="s">
+        <v>33</v>
+      </c>
+      <c r="H2" s="6" t="s">
+        <v>32</v>
+      </c>
+      <c r="I2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="J2" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="BC2" s="8"/>
     </row>
-    <row r="3" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A3" s="6">
+    <row r="3" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A3" s="3">
         <v>1024</v>
       </c>
-      <c r="B3" s="7" t="s">
+      <c r="B3" s="4" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="8" t="s">
+      <c r="C3" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="6"/>
-      <c r="E3" s="6" t="s">
+      <c r="E3" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F3" s="6" t="s">
+        <v>36</v>
+      </c>
+      <c r="G3" s="6" t="s">
+        <v>37</v>
+      </c>
+      <c r="J3" s="6" t="s">
+        <v>38</v>
+      </c>
     </row>
-    <row r="4" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A4" s="6">
+    <row r="4" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A4" s="3">
         <v>1025</v>
       </c>
-      <c r="B4" s="7" t="s">
+      <c r="B4" s="4" t="s">
         <v>1</v>
       </c>
-      <c r="C4" s="8" t="s">
+      <c r="C4" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="D4" s="6"/>
-      <c r="E4" s="6" t="s">
+      <c r="E4" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F4" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="J4" s="6" t="s">
+        <v>41</v>
+      </c>
     </row>
-    <row r="5" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A5" s="6">
+    <row r="5" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A5" s="3">
         <v>1046</v>
       </c>
-      <c r="B5" s="7" t="s">
+      <c r="B5" s="4" t="s">
         <v>2</v>
       </c>
-      <c r="C5" s="8" t="s">
+      <c r="C5" s="5" t="s">
         <v>11</v>
       </c>
-      <c r="D5" s="6"/>
-      <c r="E5" s="6" t="s">
+      <c r="E5" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F5" s="6" t="s">
+        <v>42</v>
+      </c>
+      <c r="G5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="H5" s="6" t="s">
+        <v>45</v>
+      </c>
+      <c r="J5" s="6" t="s">
+        <v>44</v>
+      </c>
     </row>
-    <row r="6" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A6" s="6">
+    <row r="6" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A6" s="3">
         <v>1056</v>
       </c>
-      <c r="B6" s="7" t="s">
+      <c r="B6" s="4" t="s">
         <v>3</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="5" t="s">
         <v>12</v>
       </c>
-      <c r="D6" s="10" t="s">
+      <c r="D6" s="7" t="s">
         <v>22</v>
       </c>
-      <c r="E6" s="6" t="s">
+      <c r="E6" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F6" s="6" t="s">
+        <v>46</v>
+      </c>
+      <c r="G6" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="H6" s="6" t="s">
+        <v>48</v>
+      </c>
+      <c r="J6" s="6" t="s">
+        <v>49</v>
+      </c>
     </row>
-    <row r="7" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A7" s="6">
+    <row r="7" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A7" s="3">
         <v>1062</v>
       </c>
-      <c r="B7" s="7" t="s">
+      <c r="B7" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="C7" s="8" t="s">
+      <c r="C7" s="5" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="10" t="s">
+      <c r="D7" s="7" t="s">
         <v>17</v>
       </c>
-      <c r="E7" s="6" t="s">
+      <c r="E7" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F7" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="G7" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="H7" s="6" t="s">
+        <v>52</v>
+      </c>
+      <c r="J7" s="6" t="s">
+        <v>53</v>
+      </c>
     </row>
-    <row r="8" spans="1:5" ht="13.2" x14ac:dyDescent="0.25">
-      <c r="A8" s="6">
+    <row r="8" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+      <c r="A8" s="3">
         <v>1066</v>
       </c>
-      <c r="B8" s="7" t="s">
+      <c r="B8" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="C8" s="8" t="s">
+      <c r="C8" s="5" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="10" t="s">
+      <c r="D8" s="7" t="s">
         <v>20</v>
       </c>
-      <c r="E8" s="6" t="s">
+      <c r="E8" s="3" t="s">
         <v>26</v>
       </c>
+      <c r="F8" s="6" t="s">
+        <v>54</v>
+      </c>
+      <c r="G8" s="6" t="s">
+        <v>55</v>
+      </c>
+      <c r="H8" s="6" t="s">
+        <v>56</v>
+      </c>
+      <c r="J8" s="6" t="s">
+        <v>57</v>
+      </c>
     </row>
-    <row r="9" spans="1:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="6">
+    <row r="9" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A9" s="3">
         <v>1067</v>
       </c>
-      <c r="B9" s="7" t="s">
+      <c r="B9" s="4" t="s">
         <v>24</v>
       </c>
-      <c r="C9" s="8" t="s">
+      <c r="C9" s="5" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="10" t="s">
+      <c r="D9" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="E9" s="9" t="s">
+      <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
+      <c r="F9" s="6" t="s">
+        <v>58</v>
+      </c>
+      <c r="G9" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="H9" s="6" t="s">
+        <v>60</v>
+      </c>
+      <c r="I9" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="J9" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="K9" s="6"/>
+      <c r="L9" s="6"/>
+      <c r="M9" s="6"/>
+      <c r="N9" s="6"/>
+      <c r="O9" s="6"/>
+      <c r="P9" s="6"/>
+      <c r="Q9" s="6"/>
+      <c r="R9" s="6"/>
+      <c r="S9" s="6"/>
+      <c r="T9" s="6"/>
+      <c r="U9" s="6"/>
+      <c r="V9" s="6"/>
+      <c r="W9" s="6"/>
+      <c r="X9" s="6"/>
+      <c r="Y9" s="6"/>
+      <c r="Z9" s="6"/>
+      <c r="AA9" s="6"/>
+      <c r="AB9" s="6"/>
+      <c r="AC9" s="6"/>
+      <c r="AD9" s="6"/>
+      <c r="AE9" s="6"/>
+      <c r="AF9" s="6"/>
+      <c r="AG9" s="6"/>
+      <c r="AH9" s="6"/>
+      <c r="AI9" s="6"/>
+      <c r="AJ9" s="6"/>
+      <c r="AK9" s="6"/>
+      <c r="AL9" s="6"/>
+      <c r="AM9" s="6"/>
+      <c r="AN9" s="6"/>
+      <c r="AO9" s="6"/>
+      <c r="AP9" s="6"/>
+      <c r="AQ9" s="6"/>
+      <c r="AR9" s="6"/>
+      <c r="AS9" s="6"/>
+      <c r="AT9" s="6"/>
+      <c r="AU9" s="6"/>
+      <c r="AV9" s="6"/>
+      <c r="AW9" s="6"/>
+      <c r="AX9" s="6"/>
+      <c r="AY9" s="6"/>
+      <c r="AZ9" s="6"/>
+      <c r="BA9" s="6"/>
+      <c r="BB9" s="6"/>
+    </row>
+    <row r="40" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="E40" s="8"/>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>
@@ -605,8 +923,39 @@
     <hyperlink ref="D6" r:id="rId4" xr:uid="{4E8EAD22-6C22-423C-B890-53F1D5FAD402}"/>
     <hyperlink ref="D9" r:id="rId5" xr:uid="{80AC4A8A-9314-4C3A-BC05-2112C8CEE699}"/>
     <hyperlink ref="E9" r:id="rId6" xr:uid="{7C602A97-F4B1-4610-AAEF-993F9E82CC57}"/>
+    <hyperlink ref="H2" r:id="rId7" xr:uid="{BDFCC72F-133F-422A-B7BE-23DEDB076016}"/>
+    <hyperlink ref="F2" r:id="rId8" xr:uid="{8F26E26E-6197-4892-98F7-CFBE1ACAF9A6}"/>
+    <hyperlink ref="J2" r:id="rId9" xr:uid="{768DBFD4-8ED3-422B-B2A0-ACE004223C29}"/>
+    <hyperlink ref="I2" r:id="rId10" xr:uid="{0EF326A8-7605-4612-B60E-51E0C40801EF}"/>
+    <hyperlink ref="F3" r:id="rId11" xr:uid="{AC3E033B-E97B-47D3-8AC8-EEF4CC7A56A1}"/>
+    <hyperlink ref="G3" r:id="rId12" xr:uid="{BD2EE1D2-6AD0-4D0C-BD88-FB70B0672A0A}"/>
+    <hyperlink ref="J3" r:id="rId13" xr:uid="{293341F4-240C-4D6F-B47F-95B4A8703BC8}"/>
+    <hyperlink ref="F4" r:id="rId14" xr:uid="{17C345FA-41BE-4865-9914-2FD9675B5B63}"/>
+    <hyperlink ref="G4" r:id="rId15" xr:uid="{4E336FC2-40EE-4CE2-B9DC-6E3D75655073}"/>
+    <hyperlink ref="J4" r:id="rId16" xr:uid="{5D074A40-A206-4281-AD49-7C2A35CFB497}"/>
+    <hyperlink ref="F5" r:id="rId17" xr:uid="{B787E1DA-41E1-44A2-985C-643F4100DBF5}"/>
+    <hyperlink ref="G5" r:id="rId18" xr:uid="{BBBF1CB8-B5C1-474F-A507-9B9DF04349AA}"/>
+    <hyperlink ref="J5" r:id="rId19" xr:uid="{F6325029-12A9-41D5-9590-E86272B0B31C}"/>
+    <hyperlink ref="H5" r:id="rId20" xr:uid="{FBF5560D-8E5C-4407-8CCD-C2509DDB57DA}"/>
+    <hyperlink ref="F6" r:id="rId21" xr:uid="{635502E2-B5C2-4594-8ED2-A018CDD8A62C}"/>
+    <hyperlink ref="G6" r:id="rId22" xr:uid="{C5D7E843-8BAA-4721-A2B6-1B29C9178473}"/>
+    <hyperlink ref="H6" r:id="rId23" xr:uid="{ABF82DA3-6FF2-4A64-9F7A-87C9911F5960}"/>
+    <hyperlink ref="J6" r:id="rId24" xr:uid="{A7DD96CC-53BB-408D-9209-BD8C8A9CFE06}"/>
+    <hyperlink ref="F7" r:id="rId25" xr:uid="{8F943837-0130-4E52-8835-F1879ED93751}"/>
+    <hyperlink ref="G7" r:id="rId26" xr:uid="{BBE2C64B-072E-41E5-B117-395CB96E4815}"/>
+    <hyperlink ref="H7" r:id="rId27" xr:uid="{C485E0BD-486C-41EC-BAD6-FCC2859FEAF0}"/>
+    <hyperlink ref="J7" r:id="rId28" xr:uid="{A5183E5D-ABA2-48E3-AE24-51D0800296A4}"/>
+    <hyperlink ref="F8" r:id="rId29" xr:uid="{0D4FFE50-E02E-4685-B931-F5888BFC3A29}"/>
+    <hyperlink ref="G8" r:id="rId30" xr:uid="{C4D52FF3-BA87-4CB3-8F59-F2393E516A95}"/>
+    <hyperlink ref="H8" r:id="rId31" xr:uid="{0273961F-0917-4A86-872D-321EE0CCDC13}"/>
+    <hyperlink ref="J8" r:id="rId32" xr:uid="{823CCC18-BF60-4301-9CF1-68447DC1E271}"/>
+    <hyperlink ref="F9" r:id="rId33" xr:uid="{BDBF79B2-FCBA-465E-A67B-504943F07CC7}"/>
+    <hyperlink ref="G9" r:id="rId34" xr:uid="{1AC387CB-9D6A-4D07-A779-7B5EEE879C39}"/>
+    <hyperlink ref="H9" r:id="rId35" xr:uid="{15242279-2DA5-483C-89AC-48D4396B67FE}"/>
+    <hyperlink ref="I9" r:id="rId36" xr:uid="{FA97C170-F7E2-4C1C-B780-52595018F460}"/>
+    <hyperlink ref="J9" r:id="rId37" xr:uid="{31D6FFDB-9EB4-4F7E-9068-82BDCC483B1B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId7"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId38"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adding another sheet to the excel
</commit_message>
<xml_diff>
--- a/test.xlsx
+++ b/test.xlsx
@@ -8,19 +8,30 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\guysh\ParserTest\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{0D005D68-961A-42A9-9ADC-D07B746691A5}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473A5566-55AD-4857-9498-4D30DB4F15F4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Part list" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="157" uniqueCount="144">
   <si>
     <t>DC ELECTRIC PANEL</t>
   </si>
@@ -209,13 +220,256 @@
   </si>
   <si>
     <t>https://www.onsight.tech/virtual-tours/BC-Draft/cardtemp/fischr/photo/Generator-fischer-panda-8000i-pms_Photo.pdf</t>
+  </si>
+  <si>
+    <t>A/C Panel Fwd.Cabin</t>
+  </si>
+  <si>
+    <t>A/C Panel Saloon</t>
+  </si>
+  <si>
+    <t>A/C Unit Fw. Cabin</t>
+  </si>
+  <si>
+    <t>A/C Unit Saloon</t>
+  </si>
+  <si>
+    <t>A/C water pump inlet + Stainer</t>
+  </si>
+  <si>
+    <t>Anchor</t>
+  </si>
+  <si>
+    <t>Auto Pilot Motor</t>
+  </si>
+  <si>
+    <t>Batteries Charger &amp; Main Breker locker</t>
+  </si>
+  <si>
+    <t>BBQ</t>
+  </si>
+  <si>
+    <t>Bilge &amp; A/C pump</t>
+  </si>
+  <si>
+    <t>Bow Thruster</t>
+  </si>
+  <si>
+    <t>Bow Thruster Battery &amp; Charger</t>
+  </si>
+  <si>
+    <t>Chart Table</t>
+  </si>
+  <si>
+    <t>Coachroof rope clutch</t>
+  </si>
+  <si>
+    <t>DC &amp; AC Panel</t>
+  </si>
+  <si>
+    <t>Engine</t>
+  </si>
+  <si>
+    <t>Engine Main Switch</t>
+  </si>
+  <si>
+    <t>Freezer</t>
+  </si>
+  <si>
+    <t>Fresh Water Manifold &amp; Pump</t>
+  </si>
+  <si>
+    <t>Fresh Water Tank Fw</t>
+  </si>
+  <si>
+    <t>Fresh Water Tank STB.</t>
+  </si>
+  <si>
+    <t>Fuel Tank-Port</t>
+  </si>
+  <si>
+    <t>Fuel Tank-STB</t>
+  </si>
+  <si>
+    <t>FWD Cabin</t>
+  </si>
+  <si>
+    <t>FWD HEAD</t>
+  </si>
+  <si>
+    <t>FWD SHOWER</t>
+  </si>
+  <si>
+    <t>Galley</t>
+  </si>
+  <si>
+    <t>GEN LAZARET</t>
+  </si>
+  <si>
+    <t>Helm &amp; Control Station</t>
+  </si>
+  <si>
+    <t>Jib Roller Deck</t>
+  </si>
+  <si>
+    <t>Pasarela Hudraulic &amp; Motor Unit</t>
+  </si>
+  <si>
+    <t>PORT HEAD</t>
+  </si>
+  <si>
+    <t>Sail &amp; Chain Locker</t>
+  </si>
+  <si>
+    <t>Services Battery</t>
+  </si>
+  <si>
+    <t>STB HEAD</t>
+  </si>
+  <si>
+    <t>Termal Switch winch&amp;Gangway</t>
+  </si>
+  <si>
+    <t>Toilet Locker Fwd</t>
+  </si>
+  <si>
+    <t>Toilet Locker Port Aft</t>
+  </si>
+  <si>
+    <t>Toilet Locker STB. Aft</t>
+  </si>
+  <si>
+    <t>Winch Elctric Switch</t>
+  </si>
+  <si>
+    <t>Windless Motor &amp;Gear</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>List</t>
+  </si>
+  <si>
+    <t>#media-name=masterbdtech.2&amp;focus-overlay-name=A/C Panel Fwd.Cabin</t>
+  </si>
+  <si>
+    <t>#media-name=pano11.1&amp;focus-overlay-name=tocard-mobile</t>
+  </si>
+  <si>
+    <t>#media-name=masterbdtech.2&amp;focus-overlay-name=A/C Unit Fw. Cabin</t>
+  </si>
+  <si>
+    <t>#media-index=maihall1.3&amp;trigger-overlay-name=maihall1.3</t>
+  </si>
+  <si>
+    <t>#media-index=mainhall1.1&amp;trigger-overlay-name=mainhall1.1</t>
+  </si>
+  <si>
+    <t>#media-name=pano1&amp;focus-overlay-name=Anchor</t>
+  </si>
+  <si>
+    <t>#media-index=mainhall.1&amp;trigger-overlay-name=mainhall.1</t>
+  </si>
+  <si>
+    <t>#media-index=pano7.1.1&amp;trigger-overlay-name=pano7.1.1</t>
+  </si>
+  <si>
+    <t>#media-name=prow.4&amp;focus-overlay-name=Bow Thruster</t>
+  </si>
+  <si>
+    <t>#media-name=masterbdtech.2&amp;focus-overlay-name=Bow Thruster Battery &amp; Charger</t>
+  </si>
+  <si>
+    <t>#media-index=&amp;trigger-overlay-name=</t>
+  </si>
+  <si>
+    <t>#media-name=radio&amp;focus-overlay-name=Chart Table</t>
+  </si>
+  <si>
+    <t>#media-name=pano4&amp;focus-overlay-name=Coachroof rope clutch</t>
+  </si>
+  <si>
+    <t>#media-index=radio&amp;trigger-overlay-name=radio</t>
+  </si>
+  <si>
+    <t>#media-name=mainhall.engine&amp;focus-overlay-name=mainhall.engine</t>
+  </si>
+  <si>
+    <t>#media-name=mainhall.1.5&amp;focus-overlay-name=Engine Main Switch</t>
+  </si>
+  <si>
+    <t>#media-index=mainhall.1.4&amp;trigger-overlay-name=mainhall.1.4</t>
+  </si>
+  <si>
+    <t>#media-index=mainhall1.2&amp;trigger-overlay-name=mainhall1.2</t>
+  </si>
+  <si>
+    <t>#media-index=masterbdtech.2&amp;trigger-overlay-name=masterbdtech.2</t>
+  </si>
+  <si>
+    <t>#media-name=mainhall2.1&amp;focus-overlay-name=Engine Main Switch</t>
+  </si>
+  <si>
+    <t>#media-name=masterbd2tech.3&amp;focus-overlay-name=Fuel Tank-Port</t>
+  </si>
+  <si>
+    <t>#media-name=bdtech.2&amp;focus-overlay-name=Fuel Tank-STB</t>
+  </si>
+  <si>
+    <t>#media-index=masterbd&amp;trigger-overlay-name=masterbd</t>
+  </si>
+  <si>
+    <t>#media-name=masterbd.1&amp;focus-overlay-name=FWD SHOWER</t>
+  </si>
+  <si>
+    <t>#media-index=pano12&amp;trigger-overlay-name=pano12</t>
+  </si>
+  <si>
+    <t>#media-index=engineoutbase&amp;trigger-overlay-name=engineoutbase</t>
+  </si>
+  <si>
+    <t>#media-index=enginein2&amp;trigger-overlay-name=enginein2</t>
+  </si>
+  <si>
+    <t>#media-name=pano7.1&amp;trigger-overlay-name=pano7.1</t>
+  </si>
+  <si>
+    <t>#media-name=prow.2&amp;focus-overlay-name=Jib Roller Deck</t>
+  </si>
+  <si>
+    <t>#media-index=engine4&amp;trigger-overlay-name=engine4</t>
+  </si>
+  <si>
+    <t>#media-name=masterbd2.3&amp;focus-overlay-name=Port Head</t>
+  </si>
+  <si>
+    <t>#media-name=prow.2&amp;focus-overlay-name=Sail &amp; Chain Locker</t>
+  </si>
+  <si>
+    <t>#media-index=mainhall.1.3&amp;trigger-overlay-name=mainhall.1.3</t>
+  </si>
+  <si>
+    <t>#media-index=bd.2&amp;trigger-overlay-name=bd.2</t>
+  </si>
+  <si>
+    <t>#media-name=bdtch.1&amp;focus-overlay-name=Termal Switch winch&amp;Gangway</t>
+  </si>
+  <si>
+    <t>#media-index=bdtech.3&amp;trigger-overlay-name=bdtech.3</t>
+  </si>
+  <si>
+    <t>#medi-name=mainhall.1.2&amp;focus-overlay-name=Winch Elctric Switch</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -250,6 +504,18 @@
       <b/>
       <sz val="10"/>
       <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF333333"/>
+      <name val="OpenSans"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF666666"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -308,7 +574,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="15">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="3" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -329,6 +595,15 @@
     <xf numFmtId="0" fontId="5" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -550,11 +825,11 @@
   </sheetPr>
   <dimension ref="A1:BC40"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+    <sheetView zoomScale="84" zoomScaleNormal="84" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="14.44140625" defaultRowHeight="15.75" customHeight="1"/>
   <cols>
     <col min="1" max="1" width="14.44140625" style="3"/>
     <col min="2" max="2" width="34.21875" style="4" customWidth="1"/>
@@ -569,7 +844,7 @@
     <col min="11" max="16384" width="14.44140625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:55" s="8" customFormat="1" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:55" s="8" customFormat="1" ht="13.2">
       <c r="A1" s="1" t="s">
         <v>15</v>
       </c>
@@ -646,7 +921,7 @@
       <c r="BB1" s="2"/>
       <c r="BC1" s="3"/>
     </row>
-    <row r="2" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:55" ht="15.75" customHeight="1">
       <c r="A2" s="3">
         <v>1009</v>
       </c>
@@ -676,7 +951,7 @@
       </c>
       <c r="BC2" s="8"/>
     </row>
-    <row r="3" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:55" ht="13.2">
       <c r="A3" s="3">
         <v>1024</v>
       </c>
@@ -699,7 +974,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="4" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:55" ht="13.2">
       <c r="A4" s="3">
         <v>1025</v>
       </c>
@@ -722,7 +997,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:55" ht="13.2">
       <c r="A5" s="3">
         <v>1046</v>
       </c>
@@ -748,7 +1023,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="6" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:55" ht="13.2">
       <c r="A6" s="3">
         <v>1056</v>
       </c>
@@ -777,7 +1052,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="7" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:55" ht="13.2">
       <c r="A7" s="3">
         <v>1062</v>
       </c>
@@ -806,7 +1081,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="8" spans="1:55" ht="13.2" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:55" ht="13.2">
       <c r="A8" s="3">
         <v>1066</v>
       </c>
@@ -835,7 +1110,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="9" spans="1:55" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:55" ht="15.75" customHeight="1">
       <c r="A9" s="3">
         <v>1067</v>
       </c>
@@ -851,7 +1126,7 @@
       <c r="E9" s="6" t="s">
         <v>26</v>
       </c>
-      <c r="F9" s="6" t="s">
+      <c r="F9" s="10" t="s">
         <v>58</v>
       </c>
       <c r="G9" s="6" t="s">
@@ -911,7 +1186,7 @@
       <c r="BA9" s="6"/>
       <c r="BB9" s="6"/>
     </row>
-    <row r="40" spans="5:5" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="5:5" ht="15.75" customHeight="1">
       <c r="E40" s="8"/>
     </row>
   </sheetData>
@@ -949,13 +1224,512 @@
     <hyperlink ref="G8" r:id="rId30" xr:uid="{C4D52FF3-BA87-4CB3-8F59-F2393E516A95}"/>
     <hyperlink ref="H8" r:id="rId31" xr:uid="{0273961F-0917-4A86-872D-321EE0CCDC13}"/>
     <hyperlink ref="J8" r:id="rId32" xr:uid="{823CCC18-BF60-4301-9CF1-68447DC1E271}"/>
-    <hyperlink ref="F9" r:id="rId33" xr:uid="{BDBF79B2-FCBA-465E-A67B-504943F07CC7}"/>
-    <hyperlink ref="G9" r:id="rId34" xr:uid="{1AC387CB-9D6A-4D07-A779-7B5EEE879C39}"/>
-    <hyperlink ref="H9" r:id="rId35" xr:uid="{15242279-2DA5-483C-89AC-48D4396B67FE}"/>
-    <hyperlink ref="I9" r:id="rId36" xr:uid="{FA97C170-F7E2-4C1C-B780-52595018F460}"/>
-    <hyperlink ref="J9" r:id="rId37" xr:uid="{31D6FFDB-9EB4-4F7E-9068-82BDCC483B1B}"/>
+    <hyperlink ref="G9" r:id="rId33" xr:uid="{1AC387CB-9D6A-4D07-A779-7B5EEE879C39}"/>
+    <hyperlink ref="H9" r:id="rId34" xr:uid="{15242279-2DA5-483C-89AC-48D4396B67FE}"/>
+    <hyperlink ref="I9" r:id="rId35" xr:uid="{FA97C170-F7E2-4C1C-B780-52595018F460}"/>
+    <hyperlink ref="J9" r:id="rId36" xr:uid="{31D6FFDB-9EB4-4F7E-9068-82BDCC483B1B}"/>
+    <hyperlink ref="F9" r:id="rId37" xr:uid="{BCD3DC6A-7EF0-4656-8AF4-9B0083FD4E0B}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId38"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E65D9A9-1B09-461E-AA80-F11A199E574A}">
+  <dimension ref="A1:C45"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C30" sqref="C30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.2"/>
+  <cols>
+    <col min="2" max="2" width="27.88671875" customWidth="1"/>
+    <col min="3" max="3" width="99" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3">
+      <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C1" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="11" t="s">
+        <v>63</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="11" t="s">
+        <v>64</v>
+      </c>
+      <c r="C3" s="14" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="11" t="s">
+        <v>65</v>
+      </c>
+      <c r="C4" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="11" t="s">
+        <v>66</v>
+      </c>
+      <c r="C5" s="14" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="11" t="s">
+        <v>67</v>
+      </c>
+      <c r="C6" s="14" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="11" t="s">
+        <v>68</v>
+      </c>
+      <c r="C7" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="11" t="s">
+        <v>69</v>
+      </c>
+      <c r="C8" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>70</v>
+      </c>
+      <c r="C9" s="14" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10">
+        <v>9</v>
+      </c>
+      <c r="B10" s="11" t="s">
+        <v>71</v>
+      </c>
+      <c r="C10" s="14" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3">
+      <c r="A11">
+        <v>10</v>
+      </c>
+      <c r="B11" s="11" t="s">
+        <v>72</v>
+      </c>
+      <c r="C11" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>73</v>
+      </c>
+      <c r="C12" s="14" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" s="11" t="s">
+        <v>74</v>
+      </c>
+      <c r="C13" s="14" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="B14" s="11" t="s">
+        <v>75</v>
+      </c>
+      <c r="C14" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3">
+      <c r="A15">
+        <v>14</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>76</v>
+      </c>
+      <c r="C15" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3">
+      <c r="A16">
+        <v>15</v>
+      </c>
+      <c r="B16" s="11" t="s">
+        <v>77</v>
+      </c>
+      <c r="C16" s="14" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="1:3">
+      <c r="A17">
+        <v>16</v>
+      </c>
+      <c r="B17" s="11" t="s">
+        <v>78</v>
+      </c>
+      <c r="C17" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="18" spans="1:3">
+      <c r="A18">
+        <v>17</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>79</v>
+      </c>
+      <c r="C18" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="19" spans="1:3">
+      <c r="A19">
+        <v>18</v>
+      </c>
+      <c r="B19" s="11" t="s">
+        <v>80</v>
+      </c>
+      <c r="C19" s="14" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="20" spans="1:3">
+      <c r="A20">
+        <v>19</v>
+      </c>
+      <c r="B20" s="11" t="s">
+        <v>81</v>
+      </c>
+      <c r="C20" s="14" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="21" spans="1:3">
+      <c r="A21">
+        <v>20</v>
+      </c>
+      <c r="B21" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="C21" s="14" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="22" spans="1:3">
+      <c r="A22">
+        <v>21</v>
+      </c>
+      <c r="B22" s="11" t="s">
+        <v>83</v>
+      </c>
+      <c r="C22" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="23" spans="1:3">
+      <c r="A23">
+        <v>22</v>
+      </c>
+      <c r="B23" s="11" t="s">
+        <v>84</v>
+      </c>
+      <c r="C23" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="24" spans="1:3">
+      <c r="A24">
+        <v>23</v>
+      </c>
+      <c r="B24" s="11" t="s">
+        <v>85</v>
+      </c>
+      <c r="C24" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="25" spans="1:3">
+      <c r="A25">
+        <v>24</v>
+      </c>
+      <c r="B25" s="11" t="s">
+        <v>86</v>
+      </c>
+      <c r="C25" s="14" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="26" spans="1:3">
+      <c r="A26">
+        <v>25</v>
+      </c>
+      <c r="B26" s="11" t="s">
+        <v>87</v>
+      </c>
+      <c r="C26" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="27" spans="1:3">
+      <c r="A27">
+        <v>26</v>
+      </c>
+      <c r="B27" s="11" t="s">
+        <v>88</v>
+      </c>
+      <c r="C27" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3">
+      <c r="A28">
+        <v>27</v>
+      </c>
+      <c r="B28" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="C28" s="14" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3">
+      <c r="A29">
+        <v>28</v>
+      </c>
+      <c r="B29" s="11" t="s">
+        <v>90</v>
+      </c>
+      <c r="C29" s="14" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3">
+      <c r="A30">
+        <v>29</v>
+      </c>
+      <c r="B30" s="11" t="s">
+        <v>24</v>
+      </c>
+      <c r="C30" s="14" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="31" spans="1:3">
+      <c r="A31">
+        <v>30</v>
+      </c>
+      <c r="B31" s="11" t="s">
+        <v>91</v>
+      </c>
+      <c r="C31" s="14" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="32" spans="1:3">
+      <c r="A32">
+        <v>31</v>
+      </c>
+      <c r="B32" s="11" t="s">
+        <v>92</v>
+      </c>
+      <c r="C32" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3">
+      <c r="A33">
+        <v>32</v>
+      </c>
+      <c r="B33" s="11" t="s">
+        <v>93</v>
+      </c>
+      <c r="C33" s="14" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3">
+      <c r="A34">
+        <v>33</v>
+      </c>
+      <c r="B34" s="11" t="s">
+        <v>94</v>
+      </c>
+      <c r="C34" s="14" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3">
+      <c r="A35">
+        <v>34</v>
+      </c>
+      <c r="B35" s="11" t="s">
+        <v>95</v>
+      </c>
+      <c r="C35" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="36" spans="1:3">
+      <c r="A36">
+        <v>35</v>
+      </c>
+      <c r="B36" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="C36" s="14" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="37" spans="1:3">
+      <c r="A37">
+        <v>36</v>
+      </c>
+      <c r="B37" s="11" t="s">
+        <v>97</v>
+      </c>
+      <c r="C37" s="14" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="38" spans="1:3">
+      <c r="A38">
+        <v>37</v>
+      </c>
+      <c r="B38" s="11" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" s="14" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="39" spans="1:3">
+      <c r="A39">
+        <v>38</v>
+      </c>
+      <c r="B39" s="11" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="40" spans="1:3">
+      <c r="A40">
+        <v>39</v>
+      </c>
+      <c r="B40" s="11" t="s">
+        <v>100</v>
+      </c>
+      <c r="C40" s="14" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="41" spans="1:3">
+      <c r="A41">
+        <v>40</v>
+      </c>
+      <c r="B41" s="11" t="s">
+        <v>101</v>
+      </c>
+      <c r="C41" s="14" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="42" spans="1:3">
+      <c r="A42">
+        <v>41</v>
+      </c>
+      <c r="B42" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="C42" s="14" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="43" spans="1:3">
+      <c r="A43">
+        <v>42</v>
+      </c>
+      <c r="B43" s="11" t="s">
+        <v>103</v>
+      </c>
+      <c r="C43" s="14" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="44" spans="1:3">
+      <c r="B44" s="12"/>
+    </row>
+    <row r="45" spans="1:3">
+      <c r="B45" s="12"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>